<commit_message>
9 qrys en qry; 2 fnc de dicc y fnc rgnes en main
</commit_message>
<xml_diff>
--- a/dicionario.xlsx
+++ b/dicionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0630F84D-4B5C-4819-BF78-A30A0D3C9BA8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
+    <workbookView xWindow="-15450" yWindow="435" windowWidth="15225" windowHeight="10320" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>nom</t>
   </si>
@@ -81,6 +81,24 @@
   </si>
   <si>
     <t>Agregar 'M' para año anterior</t>
+  </si>
+  <si>
+    <t>mtoInsReg[n]</t>
+  </si>
+  <si>
+    <t>mtoInsReg[mnd][n]</t>
+  </si>
+  <si>
+    <t>mtoRubReg[n]</t>
+  </si>
+  <si>
+    <t>mtoRubReg[mnd][n]</t>
+  </si>
+  <si>
+    <t>QUERY???</t>
+  </si>
+  <si>
+    <t>M???</t>
   </si>
 </sst>
 </file>
@@ -435,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237BCF13-B66D-41E2-B442-CAD3B66AC3F0}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,21 +519,47 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
qrys trasladadas, faltan 2 funciones de dicc reg
</commit_message>
<xml_diff>
--- a/dicionario.xlsx
+++ b/dicionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0630F84D-4B5C-4819-BF78-A30A0D3C9BA8}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA751331-5C28-4682-AC71-2EA86A259BFE}"/>
   <bookViews>
-    <workbookView xWindow="-15450" yWindow="435" windowWidth="15225" windowHeight="10320" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>nom</t>
   </si>
@@ -99,13 +99,16 @@
   </si>
   <si>
     <t>M???</t>
+  </si>
+  <si>
+    <t>NOMBRE SECTORES, NACIONALES, VARIACIONES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +116,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,11 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,6 +172,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,10 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237BCF13-B66D-41E2-B442-CAD3B66AC3F0}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,104 +489,112 @@
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
qrys trasladadas, fncns reg listas (segun reporte nov)
</commit_message>
<xml_diff>
--- a/dicionario.xlsx
+++ b/dicionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA751331-5C28-4682-AC71-2EA86A259BFE}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5721AAF8-DA90-4700-8ADF-1D83440414EF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
+    <workbookView xWindow="-14970" yWindow="435" windowWidth="15225" windowHeight="10320" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>M???</t>
   </si>
   <si>
-    <t>NOMBRE SECTORES, NACIONALES, VARIACIONES</t>
+    <t>NOMBRE SECTORES, NACIONALES, VARIACIONES, AUTOMATIZAR REDONDEO</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +479,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
mes en querys como variable
</commit_message>
<xml_diff>
--- a/dicionario.xlsx
+++ b/dicionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5721AAF8-DA90-4700-8ADF-1D83440414EF}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCF8DAD-3B3A-4927-BA7C-495680D45E8C}"/>
   <bookViews>
-    <workbookView xWindow="-14970" yWindow="435" windowWidth="15225" windowHeight="10320" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>nom</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t>mtoRubReg[mnd][n]</t>
-  </si>
-  <si>
-    <t>QUERY???</t>
-  </si>
-  <si>
-    <t>M???</t>
   </si>
   <si>
     <t>NOMBRE SECTORES, NACIONALES, VARIACIONES, AUTOMATIZAR REDONDEO</t>
@@ -479,7 +473,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -549,44 +543,38 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Datos listos, unificando qrys y standarizando funciones
</commit_message>
<xml_diff>
--- a/dicionario.xlsx
+++ b/dicionario.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCF8DAD-3B3A-4927-BA7C-495680D45E8C}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56EDA8D6-8913-4926-B6CF-B2B84DCBF60D}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11040" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>nom</t>
   </si>
@@ -65,9 +66,6 @@
     <t>mtoSecRegPct[n]</t>
   </si>
   <si>
-    <t>mtoSecRegGraf</t>
-  </si>
-  <si>
     <t>totReg[mnd]</t>
   </si>
   <si>
@@ -96,13 +94,175 @@
   </si>
   <si>
     <t>NOMBRE SECTORES, NACIONALES, VARIACIONES, AUTOMATIZAR REDONDEO</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>top 3</t>
+  </si>
+  <si>
+    <t>top 3 (usd)?</t>
+  </si>
+  <si>
+    <t>ocRegCmp</t>
+  </si>
+  <si>
+    <t>ocRegCod</t>
+  </si>
+  <si>
+    <t>ocRegMot</t>
+  </si>
+  <si>
+    <t>ocRegPrv</t>
+  </si>
+  <si>
+    <t>ocReg[mnd]</t>
+  </si>
+  <si>
+    <t>top 5</t>
+  </si>
+  <si>
+    <t>top 4</t>
+  </si>
+  <si>
+    <t>mtoCAReg[mnd]</t>
+  </si>
+  <si>
+    <t>OCCAReg</t>
+  </si>
+  <si>
+    <t>M, Var</t>
+  </si>
+  <si>
+    <t>M, Dif</t>
+  </si>
+  <si>
+    <t>comprador</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>motivo</t>
+  </si>
+  <si>
+    <t>proveedor</t>
+  </si>
+  <si>
+    <t>monto</t>
+  </si>
+  <si>
+    <t>M, CLP, USD</t>
+  </si>
+  <si>
+    <t>totRegVarPlb</t>
+  </si>
+  <si>
+    <t>totRegPct</t>
+  </si>
+  <si>
+    <t>totRegMipyme</t>
+  </si>
+  <si>
+    <t>totRegMipymePct</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>top3</t>
+  </si>
+  <si>
+    <t>ocRegLnk</t>
+  </si>
+  <si>
+    <t>prvReg</t>
+  </si>
+  <si>
+    <t>prvReg[mnd]</t>
+  </si>
+  <si>
+    <t>modReg</t>
+  </si>
+  <si>
+    <t>modRegPct</t>
+  </si>
+  <si>
+    <t>modRegCLP</t>
+  </si>
+  <si>
+    <t>mtoSecRegNacGraf3años</t>
+  </si>
+  <si>
+    <t>mtoSecRegNacGrf</t>
+  </si>
+  <si>
+    <t>mtoSecRegGrf</t>
+  </si>
+  <si>
+    <t>df -&gt; dicc</t>
+  </si>
+  <si>
+    <t>df -&gt; var -&gt; dicc</t>
+  </si>
+  <si>
+    <t>moneda como var</t>
+  </si>
+  <si>
+    <t>mnda static bool</t>
+  </si>
+  <si>
+    <t>top5</t>
+  </si>
+  <si>
+    <t>insReg[mnd][n]</t>
+  </si>
+  <si>
+    <t>insReg[n]</t>
+  </si>
+  <si>
+    <t>rubReg[n]</t>
+  </si>
+  <si>
+    <t>rubReg[mnd][n]</t>
+  </si>
+  <si>
+    <t>mtoRubRegGrf</t>
+  </si>
+  <si>
+    <t>rubRegGraf</t>
+  </si>
+  <si>
+    <t>secReg[n]</t>
+  </si>
+  <si>
+    <t>secReg[mnd][n]</t>
+  </si>
+  <si>
+    <t>secRegPct[n]</t>
+  </si>
+  <si>
+    <t>secRegGrf</t>
+  </si>
+  <si>
+    <t>secRegNacGrf</t>
+  </si>
+  <si>
+    <t>secRegNacGraf3años</t>
+  </si>
+  <si>
+    <t>totCAReg[mnd]</t>
+  </si>
+  <si>
+    <t>totCARegOC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +274,31 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,12 +330,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,10 +355,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,11 +654,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237BCF13-B66D-41E2-B442-CAD3B66AC3F0}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,102 +666,371 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="5" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D31" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="F34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>9</v>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44"/>
+      <c r="F44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45"/>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -584,5 +1038,37 @@
     <mergeCell ref="A1:XFD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89DA6EB5-8487-4F2A-8ED3-F6640A6990E3}">
+  <dimension ref="A3:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
automatizado categorías año actual
</commit_message>
<xml_diff>
--- a/dicionario.xlsx
+++ b/dicionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dccpcompras-my.sharepoint.com/personal/diego_martinez_chilecompra_cl/Documents/Escritorio/Dpt Comunicaciones/Reportes Automatizados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56EDA8D6-8913-4926-B6CF-B2B84DCBF60D}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="8_{DCFF665B-7651-4EB5-9A7A-4D8764B5CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{497F6C0C-38E4-47B1-B245-17F26C610BEC}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11040" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B83BB67-302C-46AA-9DC2-030B21C28230}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -355,6 +355,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,8 +661,8 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,18 +761,18 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>